<commit_message>
universities from M to Z scraped
</commit_message>
<xml_diff>
--- a/data/ABDULLAH GÜL ÜNİVERSİTESİ-kadro.xlsx
+++ b/data/ABDULLAH GÜL ÜNİVERSİTESİ-kadro.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1528,1046 +1528,6 @@
         </is>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>AYŞEGÜL KIDIK</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>MİMARLIK FAKÜLTESİ</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>MİMARLIK BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>BAHAR ELAGÖZ TİMUR</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>MİMARLIK FAKÜLTESİ</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>MİMARLIK BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>BEHİCE ÇELİKBAŞ</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>REKTÖRLÜK</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr"/>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>BESİME CEYLAN</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>BEYZANUR GÜNEŞ</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>BORA AKİNCE</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>REKTÖRLÜK</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr"/>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>BUKET GÜNER</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>CAVİDAN YAKUPOĞLU KARAAĞAÇ</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>MÜHENDİSLİK FAKÜLTESİ</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>BİLGİSAYAR MÜHENDİSLİĞİ BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>CENGİZ ALİ SEYHUN DEMETS</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>DARYL NICHOLAS YORK</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>DEMET ŞAYLAN</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>YAŞAM VE DOĞA BİLİMLERİ FAKÜLTESİ</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>MOLEKÜLER BİYOLOJİ VE GENETİK BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>DOĞA COŞGUN</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>EBRU TELKENAROĞLU</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>ELİF ÖZKOÇ</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>REKTÖRLÜK</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr"/>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>EMRE ARTUT</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>EREN CEMİL DELİBAŞ</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>ESMA SARAYMEN</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>REKTÖRLÜK</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr"/>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>ESRA HASOĞLU</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>ESRA KILIÇARSLAN</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>REKTÖRLÜK</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr"/>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>FATMA EKİNCİ</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>FATMA EMRAY DENİZ</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>FATMA GAMZE SÖKÜCÜ</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>FATMA KÜBRA DURNA</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>FATMA NUR AYÇİÇEK</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>REKTÖRLÜK</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>ORTAK DERSLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>FATMA NUR DİNÇOĞLU</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>FURKAN BÜTÜN</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>REKTÖRLÜK</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr"/>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>GÖKHAN ATEŞ</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>MÜHENDİSLİK FAKÜLTESİ</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>MAKİNE MÜHENDİSLİĞİ BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>GÜLCAN DURAN</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>GÜLSÜM DURAN GÜLER</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>HALİLCAN KOÇAK</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>HAYDAR AKÇADAĞ</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>HİLAL DEMİREL</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>REKTÖRLÜK</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr"/>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>HÜLYA ÖZTÜRK</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>REKTÖRLÜK</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr"/>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>HÜSEYİN GÜNER</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>YAŞAM VE DOĞA BİLİMLERİ FAKÜLTESİ</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>MOLEKÜLER BİYOLOJİ VE GENETİK BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>İBRAHİM DENEME</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>REKTÖRLÜK</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr"/>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>İBRAHİM HAKAN GÖVER</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>İNSAN VE TOPLUM BİLİMLERİ FAKÜLTESİ</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>SİYASET BİLİMİ VE ULUSLARARASI İLİŞKİLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>İSMAİL VAKUR</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>KADRİYE NUR SAYKI</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>KÜBRA EROL</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>REKTÖRLÜK</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr"/>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>ABDULLAH GÜL ÜNİVERSİTESİ</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>KÜBRA KESER</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>ÖĞRETİM GÖREVLİSİ</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER YÜKSEKOKULU</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>YABANCI DİLLER BÖLÜMÜ</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>